<commit_message>
update the main file
</commit_message>
<xml_diff>
--- a/DTCP_Results_Chengalpattu_2025.xlsx
+++ b/DTCP_Results_Chengalpattu_2025.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="DTCP Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DTCP Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,606 +429,853 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>S.No</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>Application No</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>District</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Approval Type</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Permit Issue Date</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Total Fees</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Fees Details Available</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Approval No</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Approval Letter</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Approved Plan</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Demand Details</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
         <is>
           <t>Project Title</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Applicant/Owner Signature</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>Registered Engineer Name/Address</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>Registered Engineer Mail</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>Registered Engineer Phone</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>PDF Link</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>SWP/BPA/049180/2025</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Chengalpattu</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Building Plan</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>07/01/2025</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>13,779,223.00</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>PLAN SHOWING THE PROPOSED CONSTRUCTION OF HIGH RISE COMMERCIAL BUILDING CONSIST OF BASEMENT + GROUND + 3 UPPER FLOORS COMPRISED IN SURVEY No: 107B, 108/1, 109/3, 109/5, 111/1A1 &amp; 111/1B1 OF MELAKOTTAIYUR VILLAGE, VANDALUR TALUK, CHENGALPET DISTRICT.</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>For CASAGRAND MAGNUM PRIVATE LIMITED</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>P. ELANCHEZIYAN, B.Arch, M.T.P Reg. Architect CA/2003/30729</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" s="1" t="inlineStr">
-        <is>
-          <t>View PDF</t>
-        </is>
-      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>SWP/BPA/141104/2024</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Chengalpattu</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Building Plan</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>27/02/2025</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>13,478,056.00</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>PLAN SHOWING THE PROPOSED CONSTRUCTION OF STILT + 5 FLOORS WITH 93 D.UNITS AFFORDABLE HOUSING RESIDENTIAL BUILDING AT S.NOS: 69/9D1A1 &amp; 70/2A1, EAST COAST ROAD, KANATHUR REDDIKUPPAM VILLAGE, THIRUPORUR TALUK, CHENGALPET DISTRICT.</t>
-        </is>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>For SIDHARTH FOUNDATIONS AND HOUSING LIMITED</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>G.A VAMSI VARMA K, B.Arch Regd..CA/2012/55059 4th Floor, Bootstart Co-working Rishab Arcade, Sanjay Nagar Main Road, Raj Mahal Villas 2nd Stage, Bengaluru, Karnataka-560001</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>9538974027</t>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
         </is>
       </c>
       <c r="K3" s="1" t="inlineStr">
         <is>
-          <t>View PDF</t>
-        </is>
-      </c>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>3.</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>SWP/BPA/208957/2024</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Chengalpattu</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Building Plan</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>27/02/2025</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>18,278,125.00</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>PLAN SHOWING THE PROPOSED CONSTRUCTION OF INDUSTRIAL BUILDING OF PLOT NO: 6,7 &amp; 8 IN (SURVEY NUMBER 10/1pt, 2pt, 4pt, 5pt, 6pt, 11/1Apt, 1Bpt, 1C, 1D, 1E, 14pt, 15/1pt, 2Apt, 2Bpt, 2Cpt, 16pt, 17/1Fpt, 1Gpt, 1H, 1I, 1J, 2A2Bpt, 2A3Apt, 2A3Bpt, 2A4pt, 2B1, 2B2, 2B3, 2B4, 2B5, 3A, 3B, 4A, 4B, 4C, 4D AND 4Ept.) PANCHANTHIRUTHI VILLAGE, THIRUPORUR TALUK, CHENGALPATTU DISTRICT.</t>
-        </is>
-      </c>
       <c r="G4" t="inlineStr">
         <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>PLAN SHOWING THE PROPOSED CONSTRUCTION OF INDUSTRIAL BUILDING OF PLOT NO: 6, 7 &amp; 8 IN (SURVEY NUMBER 10/1pt, 2pt, 4pt, 5pt, 6pt, 11/1Apt, 1Bpt, 1C, 1D, 1E, 14pt, 15/1pt, 2Apt, 2Bpt, 2Cpt, 16pt, 17/1Fpt, 1Gpt, 1H, 1I, 1J, 2A2Bpt, 2A3Apt, 2A3Bpt, 2A4pt, 2B1, 2B2, 2B3, 2B4, 2B5, 3A, 3B, 4A, 4B, 4C, 4D AND 4Ept.) PANCHANTHIRUTHI VILLAGE, THIRUPORUR TALUK, CHENGALPATTU DISTRICT.</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
           <t>For HEADWAY PREMIER INDUSTRIES PRIVATE LIMITED Authorised Signatory</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>A.N. RAVICHANDRAN, DCE, B.E. (Civil), ME, AIV Reg. Registered Engineer Grade-1B Reg: ENG/2022/70/10000 Structural Engineer Grade-1B Reg: ENG/2022/70/10005</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>A.N. RAVICHANDRAN, DCE., B.E. (Civil), AMIE, MIE, M.II.Struct.E Chartered Engineer, Structural Consultant Registered Engineer Grade-IIB Registered Engineer/GI/2002/090100</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>mirrahbuilders@gmail.com</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>+91 9884147407</t>
-        </is>
-      </c>
-      <c r="K4" s="1" t="inlineStr">
-        <is>
-          <t>View PDF</t>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>+91-9787144777</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>4.</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>SWP/BPA/223491/2024</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Chengalpattu</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Building Plan</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>28/01/2025</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>3,133,961.00</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>PLAN SHOWING THE PROPOSED CONSTRUCTION OF DATA COMMUNICATION CENTER (COMMERCIAL BUILDING) AT PLOT NO: 42 IN APPROVED LAY OUT NO: L.P/D.T.C.P NO:76/2021 CHENGALPATTU. COMPRISED IN SURVEY NO.36/3B(Pt.), 4A(Pt.), 4B(Pt.), 5A(Pt.), 5B1(Pt.), 5B2(Pt.), 8B(Pt.), 9A(Pt.), 37/1A(Pt.), 1B(Pt.), 2A(Pt.), 2B(Pt.), 2B2(Pt.), 2B3(Pt.), 2B4(Pt.), 2B5(Pt.), 2C(Pt.), 3(Pt.), 4A1(Pt.), 4A2(Pt.), 4C, 4D1(Pt.), 4D2(Pt.), 4E1(Pt.), 5B(Pt.), 5C, 5D(Pt.), 40/1A1A(Pt.), 1A2, 1C(Pt.), 1D1, 1D2(Pt.), 1D3(Pt.), 2B1(Pt.), 2B2, 2C(Pt.), 3B, 3C1(Pt.), 3C2, 4A, 4B, 4C, 5A(Pt.), 5B(Pt.), 41/1A1(Pt.), 1B, 1C, 1D(Pt.), 2(Pt.), 3, 4, 5, 42/1(Pt.), 2A, 2B1A(Pt.), 2B1B(Pt.), 52/1A1A6(Pt.), 1B(Pt.) OF KUNNAPATTU VILLAGE, THIRUPORUR TALUK, KUNNAPATTU PANCHAYAT THIRUPORUR PANCHAYAT UNION CHENGALPATTU DISTRICT.</t>
-        </is>
-      </c>
       <c r="G5" t="inlineStr">
         <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="J5" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="K5" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>PLAN SHOWING THE PROPOSED CONSTRUCTION OF DATA COMMUNICATION CENTER (COMMERCIAL BUILDING) AT PLOT NO: 42 IN APPROVED LAY OUT NO: L.P/D.T.C.P NO:76/2021 CHENGALPATTU COMPRISED IN SURVEY NO.36/3B(Pt.), 4A(Pt.), 4B(Pt.), 5A(Pt.), 5B1(Pt.), 5B2(Pt.), 8B(Pt.), 9A(Pt.), 37/1A(Pt.), 1B(Pt.), 2A(Pt.), 2B(Pt.), 2B2(Pt.), 2B3(Pt.), 2B4(Pt.), 2B5(Pt.), 2C(Pt.), 3(Pt.), 4A1(Pt.), 4A2(Pt.), 4C, 4D1(Pt.), 4D2(Pt.), 4E1(Pt.), 5B(Pt.), 5C, 5D(Pt.), 40/1A1(Pt.), 1A2, 1C(Pt.), 1D1, 1D2(Pt.), 1D3(Pt.), 2B1(Pt.), 2B2, 2C(Pt.), 3B, 3C1(Pt.), 3C2, 4A, 4B, 4C, 5A(Pt.), 5B(Pt.), 41/1A1(Pt.), 1B, 1C, 1D(Pt.), 2(Pt.), 3, 4, 5, 42/1(Pt.), 2A, 2B1A(Pt.), 2B1B(Pt.), 52/1A1A6(Pt.), 1B(Pt.) OF KUNNAPATTU VILLAGE, THIRUPORUR TALUK, KUNNAPATTU PANCHAYAT THIRUPORUR PANCHAYAT UNION CHENGALPATTU DISTRICT.</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
           <t>For TATA COMMUNICATIONS LIMITED</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>K. JAMAL MOHIDEEN, B.Arch Registered Architect-CA/1993/7686 New .17, Old .5, 4th Street, Ashok Nagar, Chennai-600 083</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>K. JAMAL MOHIDEEN, B.Arch Registered Architect-CA/19870586 New 5A, 6th Street, Ashok Nagar, Chennai-600 083</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>cparchitect@gmail.com</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>98400 69523</t>
-        </is>
-      </c>
-      <c r="K5" s="1" t="inlineStr">
-        <is>
-          <t>View PDF</t>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>9840640253</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>5.</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>SWP/BPA/233615/2024</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>Chengalpattu</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Building Plan</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>14/02/2025</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>3,971,039.00</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>PLAN SHOWING THE EXISTING CONSTRUCTED BUILDING &amp; PROPOSED CONSTRUCTION OF INDUSTRIAL BUILDING IN S.NO:152 / 1(PART), AS PER PATTA S.NO:152/IC, PLOT NO:AIFS, MMDA INDUSTRIAL COMPLEX AT MARAMALAINAGAR, GUDDALUR VILLAGE , CHENGALPET TALUK &amp; DISTRICT.</t>
-        </is>
-      </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Ar K Rajeshkumar</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Dhinesh. T Architect CA/2019/49592 Reg TTLP/KR/AP/2019/05/001 .1/4, 1st Street, Kasturbai Nagar, Adyar, Chennai 600 020</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>PLAN SHOWING THE EXISTING CONSTRUCTED BUILDING &amp; PROPOSED CONSTRUCTION OF INDUSTRIAL BUILDING IN S.NO:152/1(PART), AS PER PATTA S.NO:152/1C, PLOT NO:AIF5, MMDA INDUSTRIAL COMPLEX AT MARAIMALAI NAGAR, GUDUVALLUR VILLAGE, CHENGALPET TALUK &amp; DISTRICT.</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Aka Rajakumar</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Dhinesh. T Architect CA/2019/43556 Reg TLR/RAY/CA/2019/05/001 1/41, SV Street, Kasturi Bai Nagar, Awell, Chennai-600041</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
         <is>
           <t>dhinesh.architect@gmail.com</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>+91 7378038000 | +91 99600 66666</t>
-        </is>
-      </c>
-      <c r="K6" s="1" t="inlineStr">
-        <is>
-          <t>View PDF</t>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>+91 73780 38000 | +91 96003 66666</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>6.</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>SWP/BPA/240909/2024</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Chengalpattu</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Building Plan</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>20/01/2025</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>3,696,915.00</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>PLAN SHOWING THE REVISED AND EXPANSION OF M/s. ARMSTRONG INTERNATIONAL PVT.LTD. BUILDING AT PLOT NO - P-46 AT MAHINDRA WORLD CITY, CHENGALPATTU, COMPRISED IN S.NO:165/3, 171/1, 171/2, 172/1, 191/3, 193/1,193/2, 197/1, 198/1, 198/2, 199/1, 199/2. OF ANJUR VILLAGE, MAHINDRA WORLD CITY, CHENGALPATTU TALUK, CHENGALPATTU DISTRICT.</t>
-        </is>
-      </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="J7" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>PLAN SHOWING THE REVISED AND EXPANSION OF M/s. ARMSTRONG INTERNATIONAL PVT.LTD. BUILDING AT PLOT NO - P-46 AT MAHINDRA WORLD CITY, CHENGALPATTU. COMPRISED IN S.NO:165/3, 171/1, 172/1, 191/1, 193/1, 193/2, 197/1, 198/1, 198/2, 199/1, 199/2 OF ANJUR VILLAGE, MAHINDRA WORLD CITY, CHENGALPATTU TALUK, CHENGALPATTU DISTRICT.</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
           <t>For ARMSTRONG INTERNATIONAL Pvt LTD, Director - Finance.</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Dhinesh.T, Architect CA/2009/49367 Reg. TVLR/RCA/Reg2/05/001 10/51, 1st Street, Kasturibai Nagar, Alwarthirunagar, Chennai 600 054</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>dhinesh.architect@gmail.com</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>+91 73730 83006 | +91 69003 66666</t>
-        </is>
-      </c>
-      <c r="K7" s="1" t="inlineStr">
-        <is>
-          <t>View PDF</t>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Dhinesh. T, Architect. CA/2009/43967 Regd. TVLR/RSE/G-1/2023/05/001 .105/11, 1st Street, Kailashnagar, Avadi, Chennai-600054</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>dhinesh.t.architect@gmail.com</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>+91 73500 83066 | +91 69003 66666</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>7.</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>SWP/BPA/270950/2025</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Chengalpattu</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Building Plan</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>03/01/2025</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>72,764,713.00</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>PLAN SHOWING THE PROPOSED CONSTRUCTION OF GROUP DEVELOPMENT FOR AFFORDABLE RESIDENTIAL APARTMENTS HIGH RISE BUILDING IN S.F.NO.18/1, 2, 3, 8A, 8B, 8C, 10; 19/1, 2, 3, 4, 6B; 23/1A, 24/1, 25/1A, 1B, 1C, 12C3B; 30/5C1A, 6B, 7A, 8, 9, 10, 12C1A, 12C1B, 12C2, 12C3, 13A1, 13B; 31/1C1A, 11,13 AT KANATHUR REDDYKUPPAM VILLAGE, TIRUPORUR TALUK, CHENGALPATTU DISTRICT.</t>
-        </is>
-      </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>For Voora Property Developers (P) Ltd. Managing Director</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>M/s. VERNEKAR ASSOCIATES PVT. LTD. . 8, 1st 'A' Main, Stag Extension ST Bed Koramangala 4th Block BANGALORE-560095 .: 40609800, Fax: 40609810</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="J8" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
       <c r="K8" s="1" t="inlineStr">
         <is>
-          <t>View PDF</t>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>PLAN SHOWING THE PROPOSED CONSTRUCTION OF GROUP DEVELOPMENT FOR AFFORDABLE RESIDENTIAL APARTMENTS HIGH RISE BUILDING IN S.F.NO.18/1, 2, 3, 8A, 10; 19/1, 2, 3, 4, 6B; 23/1A, 24/1, 25/1A, 1B, 1C, 2, 3, 4, 5, 6, 7, 8, 9A, 9B, 9C, 10; 29/12C1, 12C2, 12C3B; 30/5C1A, 6B, 7A, 8, 9, 10, 12C1A, 12C1B, 12C2, 12C3, 13A1, 13B; 31/1C1A,11,13 AT KANATHUR REDDYKUPPAM VILLAGE, TIRUPORUR TALUK, CHENGALPATTU DISTRICT.</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>For Voora Property Developers (P) Ltd.</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>M/s. Vernekar Associates Pvt. Ltd. . 8, 1st 'A' Main, Stag Extension ST Bed Koramangala 4th Block Bangalore - 560095 40609880, Fax</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>406098810</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>8.</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>SWP/BPA/325413/2024</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>Chengalpattu</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Building Plan</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>21/01/2025</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>3,323,788.00</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>PLAN SHOWING THE PROPOSED CONSTRUCTION OF INDUSTRIAL BUILDING (FORMULATIONS OF PHARMACEUTICALS) AT SIDCO INDUSTRIAL ESTATE, PLOT NO.53,54,55,82,83 &amp; 84, COMPRISED IN OLD SURVEY NO.237/10A1A1A, NEW SURVEY NO.237/27 IN ALATHUR VILLAGE, THIRUPORUR TALUK, CHENGALPATTU DISTRICT.</t>
-        </is>
-      </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>For ORCHID PHARMA LIMITED</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>B.MALLIKA, ME., (PhD) Registered Engineer Grade-II RE-II / KKDTCP / 017 / 2022 84, Kaalimann Koli Street, Pasumpon Nagar, Madurai-625003</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="J9" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
       <c r="K9" s="1" t="inlineStr">
         <is>
-          <t>View PDF</t>
-        </is>
-      </c>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>PLAN SHOWING THE PROPOSED CONSTRUCTION OF INDUSTRIAL BUILDING (FORMULATIONS OF PHARMACEUTICALS) AT SIDCO INDUSTRIAL ESTATE, PLOT NO. 53, 54, 55, 82, 83 &amp; 84, COMPRISED IN OLD SURVEY NO. 237/10A1A1A, NEW SURVEY NO. 237/27 IN ALATHUR VILLAGE, THIRUPORUR TALUK, CHENGALPATTU DISTRICT.</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>For ORCHID PHARMA LIMITED Authorised Signatory</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>B. Mallika, M.E., (PhD) Registered Engineer Grade-II RE-II / KKDTCPI / 017 / 2022 84, Kaliamman Koil Street, Pasumpon Nagar, Madurai-625003</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>9.</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>SWP/BPA/358599/2024</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Chengalpattu</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Building Plan</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>28/01/2025</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>249,081.00</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>PLAN SHOWING OFFICE BUILDING" IN STILT FLOOR &amp; HEAD ROOM (279 SQ.M B) GUDUVANCHERI VILLAGE, CHENGALPATTU DISTRICT.</t>
-        </is>
-      </c>
       <c r="G10" t="inlineStr">
         <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="J10" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="K10" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>"PROPOSED CONSTRUCTION OF AN OFFICE BUILDING" IN STILT FLOOR &amp; PLOT NOS. (B) GUDUVANCHERI VILLAGE, CHENGALPATTU DISTRICT.</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
           <t>APPLICANT</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Er. U. UMESHRAJ, B.E., Registered Engineer Grade-II (RE) RE/CA/AUA/2024/031 .32, Nasri 1st Cross Street, Ezhil Nagar Ext., Thorapadi Post, Vellore - 632 002</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Er. U. UMESHRAJ, BE, : Registered Engineer Grade-II (RE) RE/CM/Aug-2022/031 . 32, Nasar 1st Cross Street, Ezhil Nagar, Pallavaram, Chennai 600 117</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
         <is>
           <t>umeshraj1487@gmail.com</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>99440 74734</t>
-        </is>
-      </c>
-      <c r="K10" s="1" t="inlineStr">
-        <is>
-          <t>View PDF</t>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>99440 73734</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>10.</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>SWP/BPA/360192/2025</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>Chengalpattu</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Building Plan</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>30/01/2025</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>49,619,230.00</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>PLAN SHOWING THE PROPOSED ADDITIONAL CONSTRUCTION OF RESIDENTIAL HIGHRISE GROUP DEVELOPMENT BUILDING CONSISTS OF 3 BLOCKS, BLOCK 3 &amp; 6 WITH COMMON CLUB HOUSE AT BLOCKS 1, 2, &amp; 5. BLOCK 3: GROUND+13 UPPER FLOORS (25 DU); BLOCK 6: GROUND+18 UPPER FLOORS (252 DU); BLOCK 6 CLUB HOUSE: GROUND + 3 FLOORS WITH SWIMMING POOL ON THE GROUND FLOOR, TOTAL 500 DU COMPOSED IN S.NOS. 110/2A1B, 110/2A1C, 110/2A1D, 110/2A1E, 111/1C, 111/1D, 111/1E, 111/1F, 111/1G, 111/2A1, 111/2C, 112/2A2, 112/2A1, 114/C, 114/2, 117/2B, 117/2C, 117/4, 117/5, 118/1D, 118/2, 119/1, 119/2B, 119/2A, 119/4, 119/5, 122/2A, 122/1, 122/3, 122/4, 122/5, 122/6A, 122/6B, 124/1, 124/2, 124/3, 124/4, 124/5A, 124/5B, 124/5C, 124/5D, MELAKOTTAIYUR VILLAGE, VANDALUR TALUK, CHENGALPATTU DISTRICT.</t>
-        </is>
-      </c>
       <c r="G11" t="inlineStr">
         <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="J11" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="K11" s="1" t="inlineStr">
+        <is>
+          <t>Download</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>PLAN SHOWING THE PROPOSED ADDITIONAL CONSTRUCTION OF RESIDENTIAL HIGHRISE GROUP DEVELOPMENT BUILDING CONSISTING OF 3 BLOCKS, BLOCK S &amp; W: G+10 COMMERCIAL+DOUBLE BASEMENT &amp; BLOCK B: GROUND+28 UPPER FLOORS (92 DUs), BLOCK C: GROUND+20 UPPER FLOORS (225 DUs), BLOCK D: CLUB HOUSE+GROUND+3 FLOORS WITH SWIMMING POOL ON THE GROUND FLOOR, TOTALLY 509 DUs COMPOSED IN S.NOS 81/2C, 112/1, 112/5A, 112/5B, 112/6A, 112/7A, 112/7B, 112/10A, 112/10B, 112/11A, 112/11B, 112/11C1A1, 112/11C2A, 112/11C3A, 112/12A, 112/12C, 112/12A2, 112/13A, 112/13A1A, 112/13A1B, 112/13A2, 112/13A3A, 112/13A3B, 112/13A4A, 112/13A4B, 112/13B, 112/14A, 112/14B, 112/15A, 112/15B, 112/15C, 112/15D, 112/16, 112/17, 112/17A, 112/17B, 112/17C, 112/17D, 112/18B, 112/18C, 112/18D, 112/18E, 112/18F, 112/18G, OSR &amp; LINK ROAD GIFTED VIDE GIFTDEED NO:8192/2023, DATED 03/03/2023 COMPRISED IN RS.NO.112/096A, 112/098A, 112/1014B1A, 112/1016C1A2, 112/2011C. LOCATED AT MELAKOTTAIYUR VILLAGE, VANDALUR TALUK, CHENGALPATTU DISTRICT.</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
           <t>For CASAGRAND ANCHOR PRIVATE LIMITED Authorised Signatory</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>JEYAVEL GANDHAM M.S.S B.Arch. Registered Architect - CA/2008/42210</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" s="1" t="inlineStr">
-        <is>
-          <t>View PDF</t>
-        </is>
-      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>JEYAVEL GANDHAM M.S.S, B.Arch., Registered Architect - CA/2008/42210</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K6" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K7" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K8" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K9" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K10" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K11" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="J2" r:id="rId2"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K2" r:id="rId3"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I3" r:id="rId4"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="J3" r:id="rId5"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K3" r:id="rId6"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I4" r:id="rId7"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="J4" r:id="rId8"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K4" r:id="rId9"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I5" r:id="rId10"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="J5" r:id="rId11"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K5" r:id="rId12"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I6" r:id="rId13"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="J6" r:id="rId14"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K6" r:id="rId15"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I7" r:id="rId16"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="J7" r:id="rId17"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K7" r:id="rId18"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I8" r:id="rId19"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="J8" r:id="rId20"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K8" r:id="rId21"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I9" r:id="rId22"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="J9" r:id="rId23"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K9" r:id="rId24"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I10" r:id="rId25"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="J10" r:id="rId26"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K10" r:id="rId27"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I11" r:id="rId28"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="J11" r:id="rId29"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K11" r:id="rId30"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>